<commit_message>
Connexion avec le servo
</commit_message>
<xml_diff>
--- a/doc/planning/PlanningEffectif.xlsx
+++ b/doc/planning/PlanningEffectif.xlsx
@@ -282,8 +282,95 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -293,103 +380,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -675,7 +678,7 @@
   <dimension ref="C4:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,205 +687,211 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C6" s="3"/>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="4" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="6" t="s">
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C7" s="7"/>
-      <c r="D7" s="16" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="N7" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="28">
         <v>0.16666666666666666</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="19" t="s">
+      <c r="E8" s="16"/>
+      <c r="F8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="28"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="21"/>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="20" t="s">
+      <c r="D9" s="17"/>
+      <c r="E9" s="37">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="30"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="23"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="20" t="s">
+      <c r="D10" s="17"/>
+      <c r="E10" s="37">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="F10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="31"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="24"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="20" t="s">
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="31"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="24"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="20" t="s">
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="30"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="23"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="36">
+      <c r="D13" s="29">
         <v>0.16666666666666666</v>
       </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="21" t="s">
+      <c r="E13" s="29">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="34"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="27"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="11" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajout des fonctionnalité pour le servo moteur
</commit_message>
<xml_diff>
--- a/doc/planning/PlanningEffectif.xlsx
+++ b/doc/planning/PlanningEffectif.xlsx
@@ -282,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -371,6 +371,9 @@
     <xf numFmtId="20" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -392,7 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -678,7 +681,7 @@
   <dimension ref="C4:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,57 +690,57 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C6" s="32"/>
-      <c r="D6" s="34" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="35" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="36" t="s">
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C7" s="33"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="9" t="s">
         <v>9</v>
       </c>
@@ -797,14 +800,18 @@
         <v>1</v>
       </c>
       <c r="D9" s="17"/>
-      <c r="E9" s="37">
+      <c r="E9" s="30">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
+      <c r="G9" s="30">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="H9" s="30">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="I9" s="18"/>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
@@ -817,14 +824,18 @@
         <v>2</v>
       </c>
       <c r="D10" s="17"/>
-      <c r="E10" s="37">
+      <c r="E10" s="30">
         <v>0.20833333333333334</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
+      <c r="G10" s="30">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="H10" s="30">
+        <v>0.25</v>
+      </c>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
@@ -881,7 +892,9 @@
       <c r="F13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="25"/>
+      <c r="G13" s="38">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
       <c r="J13" s="25"/>

</xml_diff>

<commit_message>
Grosse modification de la doc
Ajout de commentaire dans le programme aussi :

- Classe -> SDCard
</commit_message>
<xml_diff>
--- a/doc/planning/PlanningEffectif.xlsx
+++ b/doc/planning/PlanningEffectif.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13755" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Panning effectif" sheetId="1" r:id="rId1"/>
@@ -374,6 +374,9 @@
     <xf numFmtId="20" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -394,9 +397,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -681,7 +681,7 @@
   <dimension ref="C4:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,57 +690,57 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C6" s="33"/>
-      <c r="D6" s="35" t="s">
+      <c r="C6" s="34"/>
+      <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="36" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="37" t="s">
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C7" s="34"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="9" t="s">
         <v>9</v>
       </c>
@@ -812,7 +812,9 @@
       <c r="H9" s="30">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="I9" s="18"/>
+      <c r="I9" s="30">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="22"/>
@@ -836,8 +838,12 @@
       <c r="H10" s="30">
         <v>0.25</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
+      <c r="I10" s="30">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="J10" s="30">
+        <v>0.10416666666666667</v>
+      </c>
       <c r="K10" s="18"/>
       <c r="L10" s="22"/>
       <c r="M10" s="18"/>
@@ -892,12 +898,14 @@
       <c r="F13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="38">
+      <c r="G13" s="31">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
+      <c r="J13" s="31">
+        <v>0.22916666666666666</v>
+      </c>
       <c r="K13" s="25"/>
       <c r="L13" s="26"/>
       <c r="M13" s="19"/>

</xml_diff>